<commit_message>
Delete Camp Staff implemented
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/camps.xlsx
+++ b/OOPproj2002/src/pkg_camp/camps.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="28">
   <si>
     <t>Camp Name</t>
   </si>
@@ -586,41 +586,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2">
-        <v>100</v>
-      </c>
-      <c r="G4" s="2">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="I4" t="b" s="0">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SOLID Principles + Updates
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/camps.xlsx
+++ b/OOPproj2002/src/pkg_camp/camps.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="25">
   <si>
     <t>Camp Name</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>YCHERN CT113</t>
+  </si>
+  <si>
+    <t>CT113</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,10 @@
         <v>18</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -239,6 +245,9 @@
         <v>18</v>
       </c>
       <c r="K3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s" s="0">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Co-authored-by: dragon21356 <dragon21356@users.noreply.github.com> Co-authored-by: Frizzante16 <Frizzante16@users.noreply.github.com> Co-authored-by: #MANI SENTHILNATHAN VIGNESH# <VIGNESH024@e.ntu.edu.sg>
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/camps.xlsx
+++ b/OOPproj2002/src/pkg_camp/camps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="29">
   <si>
     <t>Camp Name</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>tester2</t>
+  </si>
+  <si>
+    <t>ntu</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -558,6 +564,9 @@
       <c r="L2" t="s" s="4">
         <v>21</v>
       </c>
+      <c r="M2" t="s" s="0">
+        <v>26</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
@@ -596,6 +605,9 @@
       <c r="L3" t="s" s="4">
         <v>26</v>
       </c>
+      <c r="M3" t="s" s="0">
+        <v>26</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
@@ -633,6 +645,50 @@
       </c>
       <c r="L4" t="s" s="4">
         <v>20</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="F5" t="n" s="5">
+        <v>100.0</v>
+      </c>
+      <c r="G5" t="n" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="H5" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="I5" t="b" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s" s="4">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>